<commit_message>
handle case where we have no mapped outers
</commit_message>
<xml_diff>
--- a/ParagonFakeDataForMacroTesting.xlsx
+++ b/ParagonFakeDataForMacroTesting.xlsx
@@ -8,18 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joshua/Documents/Paragon Workflow/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52CDB8B9-1071-DA48-BB75-B6871E5151DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{913CBE35-2457-5D4C-9141-1C38FAD66E4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="35700" windowHeight="18880" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet2" sheetId="25" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="35" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="36" r:id="rId3"/>
-    <sheet name="Sheet4" sheetId="37" r:id="rId4"/>
-    <sheet name="Sheet5" sheetId="38" r:id="rId5"/>
-    <sheet name="Sheet6" sheetId="39" r:id="rId6"/>
-    <sheet name="OUTERSKEY" sheetId="7" r:id="rId7"/>
+    <sheet name="Sheet1" sheetId="35" r:id="rId1"/>
+    <sheet name="unmapped-corp" sheetId="36" r:id="rId2"/>
+    <sheet name="Sheet4" sheetId="37" r:id="rId3"/>
+    <sheet name="Sheet5" sheetId="38" r:id="rId4"/>
+    <sheet name="Sheet6" sheetId="39" r:id="rId5"/>
+    <sheet name="OUTERSKEY" sheetId="7" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -42,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1535" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1304" uniqueCount="154">
   <si>
     <t>JOSH</t>
   </si>
@@ -498,6 +497,12 @@
   </si>
   <si>
     <t>00123</t>
+  </si>
+  <si>
+    <t>F123D</t>
+  </si>
+  <si>
+    <t>this data is for testing a corp that we do not have mapped in outerskey</t>
   </si>
 </sst>
 </file>
@@ -1007,1134 +1012,6 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EEB4BA4B-9CF4-D242-BB70-DC15312DD2F5}">
-  <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:O25"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O25" sqref="A1:O25"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="1:15" ht="19" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D2">
-        <v>99901</v>
-      </c>
-      <c r="E2">
-        <v>3</v>
-      </c>
-      <c r="F2">
-        <v>43</v>
-      </c>
-      <c r="G2">
-        <v>500</v>
-      </c>
-      <c r="H2">
-        <v>4</v>
-      </c>
-      <c r="I2">
-        <v>6</v>
-      </c>
-      <c r="J2" t="s">
-        <v>4</v>
-      </c>
-      <c r="K2" t="s">
-        <v>4</v>
-      </c>
-      <c r="L2" t="s">
-        <v>28</v>
-      </c>
-      <c r="M2" t="s">
-        <v>31</v>
-      </c>
-      <c r="N2" t="s">
-        <v>1</v>
-      </c>
-      <c r="O2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D3">
-        <v>99905</v>
-      </c>
-      <c r="E3">
-        <v>44</v>
-      </c>
-      <c r="F3">
-        <v>234</v>
-      </c>
-      <c r="G3">
-        <v>2000</v>
-      </c>
-      <c r="H3">
-        <v>0</v>
-      </c>
-      <c r="J3" t="s">
-        <v>4</v>
-      </c>
-      <c r="K3" t="s">
-        <v>4</v>
-      </c>
-      <c r="L3" t="s">
-        <v>29</v>
-      </c>
-      <c r="M3" t="s">
-        <v>34</v>
-      </c>
-      <c r="N3" t="s">
-        <v>1</v>
-      </c>
-      <c r="O3" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" t="s">
-        <v>20</v>
-      </c>
-      <c r="D4">
-        <v>99908</v>
-      </c>
-      <c r="E4">
-        <v>55</v>
-      </c>
-      <c r="F4">
-        <v>435</v>
-      </c>
-      <c r="G4">
-        <v>10090</v>
-      </c>
-      <c r="H4">
-        <v>5</v>
-      </c>
-      <c r="J4" t="s">
-        <v>4</v>
-      </c>
-      <c r="K4" t="s">
-        <v>4</v>
-      </c>
-      <c r="L4" t="s">
-        <v>30</v>
-      </c>
-      <c r="M4" t="s">
-        <v>35</v>
-      </c>
-      <c r="N4" t="s">
-        <v>1</v>
-      </c>
-      <c r="O4" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" t="s">
-        <v>59</v>
-      </c>
-      <c r="C5" t="s">
-        <v>21</v>
-      </c>
-      <c r="D5">
-        <v>99921</v>
-      </c>
-      <c r="E5">
-        <v>66</v>
-      </c>
-      <c r="F5">
-        <v>324</v>
-      </c>
-      <c r="G5">
-        <v>50500</v>
-      </c>
-      <c r="H5">
-        <v>55</v>
-      </c>
-      <c r="J5" t="s">
-        <v>4</v>
-      </c>
-      <c r="K5" t="s">
-        <v>4</v>
-      </c>
-      <c r="L5" t="s">
-        <v>31</v>
-      </c>
-      <c r="M5" t="s">
-        <v>36</v>
-      </c>
-      <c r="N5" t="s">
-        <v>1</v>
-      </c>
-      <c r="O5" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6" t="s">
-        <v>2</v>
-      </c>
-      <c r="C6" t="s">
-        <v>22</v>
-      </c>
-      <c r="D6">
-        <v>99976</v>
-      </c>
-      <c r="E6">
-        <v>7773</v>
-      </c>
-      <c r="F6">
-        <v>345</v>
-      </c>
-      <c r="G6">
-        <v>68</v>
-      </c>
-      <c r="H6">
-        <v>44</v>
-      </c>
-      <c r="J6" t="s">
-        <v>4</v>
-      </c>
-      <c r="K6" t="s">
-        <v>3</v>
-      </c>
-      <c r="L6" t="s">
-        <v>32</v>
-      </c>
-      <c r="M6" t="s">
-        <v>35</v>
-      </c>
-      <c r="N6" t="s">
-        <v>1</v>
-      </c>
-      <c r="O6" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" t="s">
-        <v>68</v>
-      </c>
-      <c r="C7" t="s">
-        <v>22</v>
-      </c>
-      <c r="D7">
-        <v>30021</v>
-      </c>
-      <c r="E7">
-        <v>7773</v>
-      </c>
-      <c r="F7">
-        <v>345</v>
-      </c>
-      <c r="G7">
-        <v>68</v>
-      </c>
-      <c r="H7">
-        <v>44</v>
-      </c>
-      <c r="J7" t="s">
-        <v>45</v>
-      </c>
-      <c r="K7" t="s">
-        <v>3</v>
-      </c>
-      <c r="L7" t="s">
-        <v>32</v>
-      </c>
-      <c r="M7" t="s">
-        <v>35</v>
-      </c>
-      <c r="N7" t="s">
-        <v>1</v>
-      </c>
-      <c r="O7" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>7</v>
-      </c>
-      <c r="B8" t="s">
-        <v>69</v>
-      </c>
-      <c r="C8" t="s">
-        <v>22</v>
-      </c>
-      <c r="D8">
-        <v>30022</v>
-      </c>
-      <c r="E8">
-        <v>7773</v>
-      </c>
-      <c r="F8">
-        <v>345</v>
-      </c>
-      <c r="G8">
-        <v>68</v>
-      </c>
-      <c r="H8">
-        <v>44</v>
-      </c>
-      <c r="J8" t="s">
-        <v>45</v>
-      </c>
-      <c r="K8" t="s">
-        <v>3</v>
-      </c>
-      <c r="L8" t="s">
-        <v>32</v>
-      </c>
-      <c r="M8" t="s">
-        <v>35</v>
-      </c>
-      <c r="N8" t="s">
-        <v>1</v>
-      </c>
-      <c r="O8" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>7</v>
-      </c>
-      <c r="B9" t="s">
-        <v>70</v>
-      </c>
-      <c r="C9" t="s">
-        <v>22</v>
-      </c>
-      <c r="D9">
-        <v>30025</v>
-      </c>
-      <c r="E9">
-        <v>7773</v>
-      </c>
-      <c r="F9">
-        <v>345</v>
-      </c>
-      <c r="G9">
-        <v>68</v>
-      </c>
-      <c r="H9">
-        <v>44</v>
-      </c>
-      <c r="J9" t="s">
-        <v>45</v>
-      </c>
-      <c r="K9" t="s">
-        <v>3</v>
-      </c>
-      <c r="L9" t="s">
-        <v>32</v>
-      </c>
-      <c r="M9" t="s">
-        <v>35</v>
-      </c>
-      <c r="N9" t="s">
-        <v>1</v>
-      </c>
-      <c r="O9" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>7</v>
-      </c>
-      <c r="B10" t="s">
-        <v>9</v>
-      </c>
-      <c r="C10" t="s">
-        <v>23</v>
-      </c>
-      <c r="D10">
-        <v>99904</v>
-      </c>
-      <c r="E10">
-        <v>345</v>
-      </c>
-      <c r="F10">
-        <v>456</v>
-      </c>
-      <c r="G10">
-        <v>95</v>
-      </c>
-      <c r="H10">
-        <v>0</v>
-      </c>
-      <c r="J10" t="s">
-        <v>4</v>
-      </c>
-      <c r="K10" t="s">
-        <v>3</v>
-      </c>
-      <c r="L10" t="s">
-        <v>31</v>
-      </c>
-      <c r="M10" t="s">
-        <v>37</v>
-      </c>
-      <c r="N10" t="s">
-        <v>1</v>
-      </c>
-      <c r="O10" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>7</v>
-      </c>
-      <c r="B11" t="s">
-        <v>2</v>
-      </c>
-      <c r="C11" t="s">
-        <v>24</v>
-      </c>
-      <c r="D11">
-        <v>99983</v>
-      </c>
-      <c r="E11">
-        <v>546</v>
-      </c>
-      <c r="F11">
-        <v>67</v>
-      </c>
-      <c r="G11">
-        <v>123</v>
-      </c>
-      <c r="H11">
-        <v>123</v>
-      </c>
-      <c r="I11">
-        <v>7</v>
-      </c>
-      <c r="J11" t="s">
-        <v>4</v>
-      </c>
-      <c r="K11" t="s">
-        <v>26</v>
-      </c>
-      <c r="L11" t="s">
-        <v>31</v>
-      </c>
-      <c r="M11" t="s">
-        <v>21</v>
-      </c>
-      <c r="N11" t="s">
-        <v>1</v>
-      </c>
-      <c r="O11" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>7</v>
-      </c>
-      <c r="B12" t="s">
-        <v>10</v>
-      </c>
-      <c r="C12" t="s">
-        <v>25</v>
-      </c>
-      <c r="D12">
-        <v>99911</v>
-      </c>
-      <c r="E12">
-        <v>234</v>
-      </c>
-      <c r="F12">
-        <v>77</v>
-      </c>
-      <c r="G12">
-        <v>42090</v>
-      </c>
-      <c r="H12">
-        <v>500</v>
-      </c>
-      <c r="J12" t="s">
-        <v>4</v>
-      </c>
-      <c r="K12" t="s">
-        <v>27</v>
-      </c>
-      <c r="L12" t="s">
-        <v>33</v>
-      </c>
-      <c r="M12" t="s">
-        <v>38</v>
-      </c>
-      <c r="N12" t="s">
-        <v>1</v>
-      </c>
-      <c r="O12" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>40</v>
-      </c>
-      <c r="B13" t="s">
-        <v>41</v>
-      </c>
-      <c r="C13" t="s">
-        <v>25</v>
-      </c>
-      <c r="D13">
-        <v>80023</v>
-      </c>
-      <c r="E13">
-        <v>345</v>
-      </c>
-      <c r="F13">
-        <v>22</v>
-      </c>
-      <c r="G13">
-        <v>4500</v>
-      </c>
-      <c r="H13">
-        <v>0</v>
-      </c>
-      <c r="J13" t="s">
-        <v>45</v>
-      </c>
-      <c r="K13" t="s">
-        <v>27</v>
-      </c>
-      <c r="L13" t="s">
-        <v>33</v>
-      </c>
-      <c r="M13" t="s">
-        <v>38</v>
-      </c>
-      <c r="N13" t="s">
-        <v>1</v>
-      </c>
-      <c r="O13" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>40</v>
-      </c>
-      <c r="B14" t="s">
-        <v>42</v>
-      </c>
-      <c r="C14" t="s">
-        <v>25</v>
-      </c>
-      <c r="D14">
-        <v>80024</v>
-      </c>
-      <c r="E14">
-        <v>345</v>
-      </c>
-      <c r="F14">
-        <v>22</v>
-      </c>
-      <c r="G14">
-        <v>8000</v>
-      </c>
-      <c r="H14">
-        <v>55</v>
-      </c>
-      <c r="J14" t="s">
-        <v>45</v>
-      </c>
-      <c r="K14" t="s">
-        <v>27</v>
-      </c>
-      <c r="L14" t="s">
-        <v>33</v>
-      </c>
-      <c r="M14" t="s">
-        <v>38</v>
-      </c>
-      <c r="N14" t="s">
-        <v>1</v>
-      </c>
-      <c r="O14" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>40</v>
-      </c>
-      <c r="B15" t="s">
-        <v>43</v>
-      </c>
-      <c r="C15" t="s">
-        <v>25</v>
-      </c>
-      <c r="D15">
-        <v>80025</v>
-      </c>
-      <c r="E15">
-        <v>345</v>
-      </c>
-      <c r="F15">
-        <v>22</v>
-      </c>
-      <c r="G15">
-        <v>9500</v>
-      </c>
-      <c r="H15">
-        <v>44</v>
-      </c>
-      <c r="J15" t="s">
-        <v>45</v>
-      </c>
-      <c r="K15" t="s">
-        <v>27</v>
-      </c>
-      <c r="L15" t="s">
-        <v>33</v>
-      </c>
-      <c r="M15" t="s">
-        <v>38</v>
-      </c>
-      <c r="N15" t="s">
-        <v>1</v>
-      </c>
-      <c r="O15" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>40</v>
-      </c>
-      <c r="B16" t="s">
-        <v>67</v>
-      </c>
-      <c r="C16" t="s">
-        <v>25</v>
-      </c>
-      <c r="D16">
-        <v>80026</v>
-      </c>
-      <c r="E16">
-        <v>345</v>
-      </c>
-      <c r="F16">
-        <v>22</v>
-      </c>
-      <c r="G16">
-        <v>62</v>
-      </c>
-      <c r="H16">
-        <v>4</v>
-      </c>
-      <c r="J16" t="s">
-        <v>45</v>
-      </c>
-      <c r="K16" t="s">
-        <v>27</v>
-      </c>
-      <c r="L16" t="s">
-        <v>33</v>
-      </c>
-      <c r="M16" t="s">
-        <v>38</v>
-      </c>
-      <c r="N16" t="s">
-        <v>1</v>
-      </c>
-      <c r="O16" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>40</v>
-      </c>
-      <c r="B17" t="s">
-        <v>44</v>
-      </c>
-      <c r="C17" t="s">
-        <v>25</v>
-      </c>
-      <c r="D17">
-        <v>80027</v>
-      </c>
-      <c r="E17">
-        <v>345</v>
-      </c>
-      <c r="F17">
-        <v>22</v>
-      </c>
-      <c r="G17">
-        <v>69</v>
-      </c>
-      <c r="H17">
-        <v>4</v>
-      </c>
-      <c r="J17" t="s">
-        <v>45</v>
-      </c>
-      <c r="K17" t="s">
-        <v>27</v>
-      </c>
-      <c r="L17" t="s">
-        <v>33</v>
-      </c>
-      <c r="M17" t="s">
-        <v>38</v>
-      </c>
-      <c r="N17" t="s">
-        <v>1</v>
-      </c>
-      <c r="O17" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>46</v>
-      </c>
-      <c r="B18" t="s">
-        <v>47</v>
-      </c>
-      <c r="C18" t="s">
-        <v>25</v>
-      </c>
-      <c r="D18">
-        <v>34022</v>
-      </c>
-      <c r="E18">
-        <v>2333</v>
-      </c>
-      <c r="F18">
-        <v>2567</v>
-      </c>
-      <c r="G18">
-        <v>5343</v>
-      </c>
-      <c r="H18">
-        <v>0</v>
-      </c>
-      <c r="J18" t="s">
-        <v>4</v>
-      </c>
-      <c r="K18" t="s">
-        <v>27</v>
-      </c>
-      <c r="L18" t="s">
-        <v>33</v>
-      </c>
-      <c r="M18" t="s">
-        <v>38</v>
-      </c>
-      <c r="N18" t="s">
-        <v>1</v>
-      </c>
-      <c r="O18" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>46</v>
-      </c>
-      <c r="B19" t="s">
-        <v>47</v>
-      </c>
-      <c r="C19" t="s">
-        <v>25</v>
-      </c>
-      <c r="D19">
-        <v>34023</v>
-      </c>
-      <c r="E19">
-        <v>2333</v>
-      </c>
-      <c r="F19">
-        <v>2567</v>
-      </c>
-      <c r="G19">
-        <v>324</v>
-      </c>
-      <c r="H19">
-        <v>0</v>
-      </c>
-      <c r="J19" t="s">
-        <v>4</v>
-      </c>
-      <c r="K19" t="s">
-        <v>27</v>
-      </c>
-      <c r="L19" t="s">
-        <v>33</v>
-      </c>
-      <c r="M19" t="s">
-        <v>38</v>
-      </c>
-      <c r="N19" t="s">
-        <v>1</v>
-      </c>
-      <c r="O19" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>46</v>
-      </c>
-      <c r="B20" t="s">
-        <v>47</v>
-      </c>
-      <c r="C20" t="s">
-        <v>25</v>
-      </c>
-      <c r="D20">
-        <v>34024</v>
-      </c>
-      <c r="E20">
-        <v>2333</v>
-      </c>
-      <c r="F20">
-        <v>2567</v>
-      </c>
-      <c r="G20">
-        <v>5679</v>
-      </c>
-      <c r="H20">
-        <v>0</v>
-      </c>
-      <c r="J20" t="s">
-        <v>4</v>
-      </c>
-      <c r="K20" t="s">
-        <v>27</v>
-      </c>
-      <c r="L20" t="s">
-        <v>33</v>
-      </c>
-      <c r="M20" t="s">
-        <v>38</v>
-      </c>
-      <c r="N20" t="s">
-        <v>1</v>
-      </c>
-      <c r="O20" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
-        <v>46</v>
-      </c>
-      <c r="B21" t="s">
-        <v>47</v>
-      </c>
-      <c r="C21" t="s">
-        <v>25</v>
-      </c>
-      <c r="D21">
-        <v>34025</v>
-      </c>
-      <c r="E21">
-        <v>2333</v>
-      </c>
-      <c r="F21">
-        <v>2567</v>
-      </c>
-      <c r="G21">
-        <v>32790</v>
-      </c>
-      <c r="H21">
-        <v>0</v>
-      </c>
-      <c r="I21">
-        <v>44</v>
-      </c>
-      <c r="J21" t="s">
-        <v>4</v>
-      </c>
-      <c r="K21" t="s">
-        <v>27</v>
-      </c>
-      <c r="L21" t="s">
-        <v>33</v>
-      </c>
-      <c r="M21" t="s">
-        <v>38</v>
-      </c>
-      <c r="N21" t="s">
-        <v>1</v>
-      </c>
-      <c r="O21" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
-        <v>46</v>
-      </c>
-      <c r="B22" t="s">
-        <v>47</v>
-      </c>
-      <c r="C22" t="s">
-        <v>25</v>
-      </c>
-      <c r="D22">
-        <v>34026</v>
-      </c>
-      <c r="E22">
-        <v>2333</v>
-      </c>
-      <c r="F22">
-        <v>2567</v>
-      </c>
-      <c r="G22">
-        <v>68</v>
-      </c>
-      <c r="H22">
-        <v>0</v>
-      </c>
-      <c r="J22" t="s">
-        <v>4</v>
-      </c>
-      <c r="K22" t="s">
-        <v>27</v>
-      </c>
-      <c r="L22" t="s">
-        <v>33</v>
-      </c>
-      <c r="M22" t="s">
-        <v>38</v>
-      </c>
-      <c r="N22" t="s">
-        <v>1</v>
-      </c>
-      <c r="O22" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
-        <v>46</v>
-      </c>
-      <c r="B23" t="s">
-        <v>48</v>
-      </c>
-      <c r="C23" t="s">
-        <v>25</v>
-      </c>
-      <c r="D23">
-        <v>34027</v>
-      </c>
-      <c r="E23">
-        <v>2333</v>
-      </c>
-      <c r="F23">
-        <v>2567</v>
-      </c>
-      <c r="G23">
-        <v>190</v>
-      </c>
-      <c r="H23">
-        <v>0</v>
-      </c>
-      <c r="J23" t="s">
-        <v>4</v>
-      </c>
-      <c r="K23" t="s">
-        <v>27</v>
-      </c>
-      <c r="L23" t="s">
-        <v>33</v>
-      </c>
-      <c r="M23" t="s">
-        <v>38</v>
-      </c>
-      <c r="N23" t="s">
-        <v>1</v>
-      </c>
-      <c r="O23" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
-        <v>46</v>
-      </c>
-      <c r="B24" t="s">
-        <v>49</v>
-      </c>
-      <c r="C24" t="s">
-        <v>25</v>
-      </c>
-      <c r="D24">
-        <v>34028</v>
-      </c>
-      <c r="E24">
-        <v>2333</v>
-      </c>
-      <c r="F24">
-        <v>2567</v>
-      </c>
-      <c r="G24">
-        <v>25400</v>
-      </c>
-      <c r="H24">
-        <v>0</v>
-      </c>
-      <c r="J24" t="s">
-        <v>4</v>
-      </c>
-      <c r="K24" t="s">
-        <v>27</v>
-      </c>
-      <c r="L24" t="s">
-        <v>33</v>
-      </c>
-      <c r="M24" t="s">
-        <v>38</v>
-      </c>
-      <c r="N24" t="s">
-        <v>1</v>
-      </c>
-      <c r="O24" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
-        <v>46</v>
-      </c>
-      <c r="B25" t="s">
-        <v>50</v>
-      </c>
-      <c r="C25" t="s">
-        <v>25</v>
-      </c>
-      <c r="D25" s="15" t="s">
-        <v>151</v>
-      </c>
-      <c r="E25">
-        <v>2333</v>
-      </c>
-      <c r="F25">
-        <v>2567</v>
-      </c>
-      <c r="G25">
-        <v>798</v>
-      </c>
-      <c r="H25">
-        <v>0</v>
-      </c>
-      <c r="J25" t="s">
-        <v>4</v>
-      </c>
-      <c r="K25" t="s">
-        <v>27</v>
-      </c>
-      <c r="L25" t="s">
-        <v>33</v>
-      </c>
-      <c r="M25" t="s">
-        <v>38</v>
-      </c>
-      <c r="N25" t="s">
-        <v>1</v>
-      </c>
-      <c r="O25" t="s">
-        <v>39</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8DA4D0CC-E014-FE4E-9915-E7861F86BBF2}">
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:O25"/>
@@ -3262,18 +2139,18 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2F8BB01-9F7C-3043-8A41-43AF7377D9FA}">
   <sheetPr codeName="Sheet4"/>
-  <dimension ref="A1:O25"/>
+  <dimension ref="A1:P25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:O25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="R16" sqref="R16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:15" ht="19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" ht="19" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
@@ -3319,13 +2196,16 @@
       <c r="O1" s="1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P1" s="1" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>7</v>
       </c>
       <c r="B2" t="s">
-        <v>2</v>
+        <v>152</v>
       </c>
       <c r="C2" t="s">
         <v>18</v>
@@ -3367,12 +2247,12 @@
         <v>39</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>7</v>
       </c>
       <c r="B3" t="s">
-        <v>2</v>
+        <v>152</v>
       </c>
       <c r="C3" t="s">
         <v>19</v>
@@ -3411,12 +2291,12 @@
         <v>39</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>7</v>
       </c>
       <c r="B4" t="s">
-        <v>8</v>
+        <v>152</v>
       </c>
       <c r="C4" t="s">
         <v>20</v>
@@ -3455,12 +2335,12 @@
         <v>39</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>7</v>
       </c>
       <c r="B5" t="s">
-        <v>59</v>
+        <v>152</v>
       </c>
       <c r="C5" t="s">
         <v>21</v>
@@ -3499,12 +2379,12 @@
         <v>39</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>7</v>
       </c>
       <c r="B6" t="s">
-        <v>2</v>
+        <v>152</v>
       </c>
       <c r="C6" t="s">
         <v>22</v>
@@ -3543,12 +2423,12 @@
         <v>39</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>68</v>
+        <v>152</v>
       </c>
       <c r="C7" t="s">
         <v>22</v>
@@ -3587,12 +2467,12 @@
         <v>39</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>69</v>
+        <v>152</v>
       </c>
       <c r="C8" t="s">
         <v>22</v>
@@ -3631,12 +2511,12 @@
         <v>39</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>70</v>
+        <v>152</v>
       </c>
       <c r="C9" t="s">
         <v>22</v>
@@ -3675,12 +2555,12 @@
         <v>39</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>7</v>
       </c>
       <c r="B10" t="s">
-        <v>9</v>
+        <v>152</v>
       </c>
       <c r="C10" t="s">
         <v>23</v>
@@ -3719,12 +2599,12 @@
         <v>39</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>7</v>
       </c>
       <c r="B11" t="s">
-        <v>2</v>
+        <v>152</v>
       </c>
       <c r="C11" t="s">
         <v>24</v>
@@ -3766,12 +2646,12 @@
         <v>39</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>7</v>
       </c>
       <c r="B12" t="s">
-        <v>10</v>
+        <v>152</v>
       </c>
       <c r="C12" t="s">
         <v>25</v>
@@ -3810,12 +2690,12 @@
         <v>39</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>40</v>
       </c>
       <c r="B13" t="s">
-        <v>41</v>
+        <v>152</v>
       </c>
       <c r="C13" t="s">
         <v>25</v>
@@ -3854,12 +2734,12 @@
         <v>39</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>40</v>
       </c>
       <c r="B14" t="s">
-        <v>42</v>
+        <v>152</v>
       </c>
       <c r="C14" t="s">
         <v>25</v>
@@ -3898,12 +2778,12 @@
         <v>39</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>40</v>
       </c>
       <c r="B15" t="s">
-        <v>43</v>
+        <v>152</v>
       </c>
       <c r="C15" t="s">
         <v>25</v>
@@ -3942,12 +2822,12 @@
         <v>39</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>40</v>
       </c>
       <c r="B16" t="s">
-        <v>67</v>
+        <v>152</v>
       </c>
       <c r="C16" t="s">
         <v>25</v>
@@ -3991,7 +2871,7 @@
         <v>40</v>
       </c>
       <c r="B17" t="s">
-        <v>44</v>
+        <v>152</v>
       </c>
       <c r="C17" t="s">
         <v>25</v>
@@ -4035,7 +2915,7 @@
         <v>46</v>
       </c>
       <c r="B18" t="s">
-        <v>47</v>
+        <v>152</v>
       </c>
       <c r="C18" t="s">
         <v>25</v>
@@ -4079,7 +2959,7 @@
         <v>46</v>
       </c>
       <c r="B19" t="s">
-        <v>47</v>
+        <v>152</v>
       </c>
       <c r="C19" t="s">
         <v>25</v>
@@ -4123,7 +3003,7 @@
         <v>46</v>
       </c>
       <c r="B20" t="s">
-        <v>47</v>
+        <v>152</v>
       </c>
       <c r="C20" t="s">
         <v>25</v>
@@ -4167,7 +3047,7 @@
         <v>46</v>
       </c>
       <c r="B21" t="s">
-        <v>47</v>
+        <v>152</v>
       </c>
       <c r="C21" t="s">
         <v>25</v>
@@ -4214,7 +3094,7 @@
         <v>46</v>
       </c>
       <c r="B22" t="s">
-        <v>47</v>
+        <v>152</v>
       </c>
       <c r="C22" t="s">
         <v>25</v>
@@ -4258,7 +3138,7 @@
         <v>46</v>
       </c>
       <c r="B23" t="s">
-        <v>48</v>
+        <v>152</v>
       </c>
       <c r="C23" t="s">
         <v>25</v>
@@ -4302,7 +3182,7 @@
         <v>46</v>
       </c>
       <c r="B24" t="s">
-        <v>49</v>
+        <v>152</v>
       </c>
       <c r="C24" t="s">
         <v>25</v>
@@ -4346,7 +3226,7 @@
         <v>46</v>
       </c>
       <c r="B25" t="s">
-        <v>50</v>
+        <v>152</v>
       </c>
       <c r="C25" t="s">
         <v>25</v>
@@ -4390,7 +3270,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6A47EC9-6FF9-C94A-93F5-603B3A771B7A}">
   <sheetPr codeName="Sheet6"/>
   <dimension ref="A1:O25"/>
@@ -5518,7 +4398,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4813409B-7228-2F49-BA7C-B95E948D09DC}">
   <sheetPr codeName="Sheet7"/>
   <dimension ref="A1:O25"/>
@@ -6646,7 +5526,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F5EC7DD-B0EB-9B41-BA63-AAF43418DED7}">
   <sheetPr codeName="Sheet8"/>
   <dimension ref="A1:O25"/>
@@ -7774,7 +6654,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3741EEE-A7B0-834D-9676-C4A7ABC54ECC}">
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:G57"/>

</xml_diff>

<commit_message>
update excel spreadsheet for testing
</commit_message>
<xml_diff>
--- a/ParagonFakeDataForMacroTesting.xlsx
+++ b/ParagonFakeDataForMacroTesting.xlsx
@@ -1,24 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10402"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10413"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joshua/Documents/Paragon Workflow/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{913CBE35-2457-5D4C-9141-1C38FAD66E4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71539134-93A0-8448-9B16-099BDA2DF3ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="35700" windowHeight="18880" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="35700" windowHeight="18880" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="35" r:id="rId1"/>
     <sheet name="unmapped-corp" sheetId="36" r:id="rId2"/>
-    <sheet name="Sheet4" sheetId="37" r:id="rId3"/>
-    <sheet name="Sheet5" sheetId="38" r:id="rId4"/>
-    <sheet name="Sheet6" sheetId="39" r:id="rId5"/>
-    <sheet name="OUTERSKEY" sheetId="7" r:id="rId6"/>
+    <sheet name="FilteredData" sheetId="43" r:id="rId3"/>
+    <sheet name="s1" sheetId="37" r:id="rId4"/>
+    <sheet name="Sheet5" sheetId="38" r:id="rId5"/>
+    <sheet name="Sheet6" sheetId="39" r:id="rId6"/>
+    <sheet name="OUTERSKEY" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -41,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1304" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1406" uniqueCount="164">
   <si>
     <t>JOSH</t>
   </si>
@@ -503,13 +504,43 @@
   </si>
   <si>
     <t>this data is for testing a corp that we do not have mapped in outerskey</t>
+  </si>
+  <si>
+    <t>OUTER</t>
+  </si>
+  <si>
+    <t>Color Key</t>
+  </si>
+  <si>
+    <t>Remakes</t>
+  </si>
+  <si>
+    <t>C4 Outers</t>
+  </si>
+  <si>
+    <t>Work Orders Of Jobs With Inserts</t>
+  </si>
+  <si>
+    <t>Work Orders Of Jobs With Outers We Should Order (0 Inserts)</t>
+  </si>
+  <si>
+    <t>New Entries</t>
+  </si>
+  <si>
+    <t>SUM</t>
+  </si>
+  <si>
+    <t>STOCK_LOCATION</t>
+  </si>
+  <si>
+    <t>B4S21</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -551,8 +582,23 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="9">
+  <fills count="15">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -601,8 +647,44 @@
         <bgColor rgb="FFEAD1DC"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFEE8FCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF6F91"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC8C8C8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFAB60"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA4F9E8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -636,11 +718,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -679,6 +776,45 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="10" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="11" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="0" fillId="11" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="3" fontId="7" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="13" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1784,7 +1920,7 @@
         <v>46</v>
       </c>
       <c r="B18" t="s">
-        <v>47</v>
+        <v>163</v>
       </c>
       <c r="C18" t="s">
         <v>25</v>
@@ -2144,7 +2280,7 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:P25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="R16" sqref="R16"/>
     </sheetView>
   </sheetViews>
@@ -3271,12 +3407,763 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56C642B1-A0B5-1B4B-87FB-E4BE26815493}">
+  <dimension ref="A1:H43"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="8.83203125" style="17" customWidth="1"/>
+    <col min="2" max="2" width="8.83203125" customWidth="1"/>
+    <col min="3" max="3" width="8.83203125" style="16" customWidth="1"/>
+    <col min="4" max="4" width="9.33203125" customWidth="1"/>
+    <col min="5" max="5" width="8.33203125" customWidth="1"/>
+    <col min="6" max="6" width="7.33203125" customWidth="1"/>
+    <col min="7" max="7" width="3.83203125" customWidth="1"/>
+    <col min="8" max="8" width="16.83203125" style="17" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1" s="20" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="19" t="s">
+        <v>71</v>
+      </c>
+      <c r="D1" s="18" t="s">
+        <v>51</v>
+      </c>
+      <c r="E1" s="18" t="s">
+        <v>52</v>
+      </c>
+      <c r="F1" s="18" t="s">
+        <v>53</v>
+      </c>
+      <c r="G1" s="18" t="s">
+        <v>72</v>
+      </c>
+      <c r="H1" s="20" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="18" t="s">
+        <v>68</v>
+      </c>
+      <c r="C2" s="23">
+        <v>30021</v>
+      </c>
+      <c r="D2" s="21">
+        <v>68</v>
+      </c>
+      <c r="E2" s="21">
+        <v>44</v>
+      </c>
+      <c r="F2" s="21"/>
+      <c r="G2" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="H2" s="22" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="18" t="s">
+        <v>69</v>
+      </c>
+      <c r="C3" s="23">
+        <v>30022</v>
+      </c>
+      <c r="D3" s="21">
+        <v>68</v>
+      </c>
+      <c r="E3" s="21">
+        <v>44</v>
+      </c>
+      <c r="F3" s="21"/>
+      <c r="G3" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="H3" s="22" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="18" t="s">
+        <v>70</v>
+      </c>
+      <c r="C4" s="23">
+        <v>30025</v>
+      </c>
+      <c r="D4" s="21">
+        <v>68</v>
+      </c>
+      <c r="E4" s="21">
+        <v>44</v>
+      </c>
+      <c r="F4" s="21"/>
+      <c r="G4" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="H4" s="22" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5" s="20" t="s">
+        <v>46</v>
+      </c>
+      <c r="B5" s="18" t="s">
+        <v>163</v>
+      </c>
+      <c r="C5" s="40">
+        <v>34022</v>
+      </c>
+      <c r="D5" s="21">
+        <v>5343</v>
+      </c>
+      <c r="E5" s="21">
+        <v>0</v>
+      </c>
+      <c r="F5" s="21"/>
+      <c r="G5" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="H5" s="20" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6" s="20" t="s">
+        <v>46</v>
+      </c>
+      <c r="B6" s="18" t="s">
+        <v>47</v>
+      </c>
+      <c r="C6" s="19">
+        <v>34023</v>
+      </c>
+      <c r="D6" s="21">
+        <v>324</v>
+      </c>
+      <c r="E6" s="21">
+        <v>0</v>
+      </c>
+      <c r="F6" s="21"/>
+      <c r="G6" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="H6" s="20"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A7" s="20" t="s">
+        <v>46</v>
+      </c>
+      <c r="B7" s="18" t="s">
+        <v>47</v>
+      </c>
+      <c r="C7" s="19">
+        <v>34024</v>
+      </c>
+      <c r="D7" s="21">
+        <v>5679</v>
+      </c>
+      <c r="E7" s="21">
+        <v>0</v>
+      </c>
+      <c r="F7" s="21"/>
+      <c r="G7" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="H7" s="20"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A8" s="27" t="s">
+        <v>46</v>
+      </c>
+      <c r="B8" s="24" t="s">
+        <v>47</v>
+      </c>
+      <c r="C8" s="25">
+        <v>34025</v>
+      </c>
+      <c r="D8" s="26">
+        <v>32790</v>
+      </c>
+      <c r="E8" s="26">
+        <v>0</v>
+      </c>
+      <c r="F8" s="26">
+        <v>44</v>
+      </c>
+      <c r="G8" s="24" t="s">
+        <v>4</v>
+      </c>
+      <c r="H8" s="27"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A9" s="20" t="s">
+        <v>46</v>
+      </c>
+      <c r="B9" s="18" t="s">
+        <v>47</v>
+      </c>
+      <c r="C9" s="19">
+        <v>34026</v>
+      </c>
+      <c r="D9" s="21">
+        <v>68</v>
+      </c>
+      <c r="E9" s="21">
+        <v>0</v>
+      </c>
+      <c r="F9" s="21"/>
+      <c r="G9" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="H9" s="20"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A10" s="20" t="s">
+        <v>46</v>
+      </c>
+      <c r="B10" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="C10" s="19">
+        <v>34027</v>
+      </c>
+      <c r="D10" s="21">
+        <v>190</v>
+      </c>
+      <c r="E10" s="21">
+        <v>0</v>
+      </c>
+      <c r="F10" s="21"/>
+      <c r="G10" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="H10" s="20"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A11" s="20" t="s">
+        <v>46</v>
+      </c>
+      <c r="B11" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="C11" s="19">
+        <v>34028</v>
+      </c>
+      <c r="D11" s="21">
+        <v>25400</v>
+      </c>
+      <c r="E11" s="21">
+        <v>0</v>
+      </c>
+      <c r="F11" s="21"/>
+      <c r="G11" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="H11" s="20"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A12" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="B12" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="C12" s="19">
+        <v>80023</v>
+      </c>
+      <c r="D12" s="21">
+        <v>4500</v>
+      </c>
+      <c r="E12" s="21">
+        <v>0</v>
+      </c>
+      <c r="F12" s="21"/>
+      <c r="G12" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="H12" s="20"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A13" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="B13" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="C13" s="23">
+        <v>80024</v>
+      </c>
+      <c r="D13" s="21">
+        <v>8000</v>
+      </c>
+      <c r="E13" s="21">
+        <v>55</v>
+      </c>
+      <c r="F13" s="21"/>
+      <c r="G13" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="H13" s="20"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A14" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="B14" s="18" t="s">
+        <v>43</v>
+      </c>
+      <c r="C14" s="23">
+        <v>80025</v>
+      </c>
+      <c r="D14" s="21">
+        <v>9500</v>
+      </c>
+      <c r="E14" s="21">
+        <v>44</v>
+      </c>
+      <c r="F14" s="21"/>
+      <c r="G14" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="H14" s="20"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A15" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="B15" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="C15" s="19">
+        <v>80026</v>
+      </c>
+      <c r="D15" s="21">
+        <v>62</v>
+      </c>
+      <c r="E15" s="21">
+        <v>4</v>
+      </c>
+      <c r="F15" s="21"/>
+      <c r="G15" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="H15" s="20"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A16" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="B16" s="18" t="s">
+        <v>44</v>
+      </c>
+      <c r="C16" s="19">
+        <v>80027</v>
+      </c>
+      <c r="D16" s="21">
+        <v>69</v>
+      </c>
+      <c r="E16" s="21">
+        <v>4</v>
+      </c>
+      <c r="F16" s="21"/>
+      <c r="G16" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="H16" s="20"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A17" s="27" t="s">
+        <v>7</v>
+      </c>
+      <c r="B17" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="C17" s="25">
+        <v>99901</v>
+      </c>
+      <c r="D17" s="26">
+        <v>500</v>
+      </c>
+      <c r="E17" s="26">
+        <v>4</v>
+      </c>
+      <c r="F17" s="26">
+        <v>6</v>
+      </c>
+      <c r="G17" s="24" t="s">
+        <v>4</v>
+      </c>
+      <c r="H17" s="27"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A18" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="B18" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="C18" s="19">
+        <v>99904</v>
+      </c>
+      <c r="D18" s="21">
+        <v>95</v>
+      </c>
+      <c r="E18" s="21">
+        <v>0</v>
+      </c>
+      <c r="F18" s="21"/>
+      <c r="G18" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="H18" s="20"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A19" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="B19" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="C19" s="19">
+        <v>99905</v>
+      </c>
+      <c r="D19" s="21">
+        <v>2000</v>
+      </c>
+      <c r="E19" s="21">
+        <v>0</v>
+      </c>
+      <c r="F19" s="21"/>
+      <c r="G19" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="H19" s="20"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A20" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="B20" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="C20" s="23">
+        <v>99908</v>
+      </c>
+      <c r="D20" s="21">
+        <v>10090</v>
+      </c>
+      <c r="E20" s="21">
+        <v>5</v>
+      </c>
+      <c r="F20" s="21"/>
+      <c r="G20" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="H20" s="20" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A21" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="B21" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="C21" s="23">
+        <v>99911</v>
+      </c>
+      <c r="D21" s="21">
+        <v>42090</v>
+      </c>
+      <c r="E21" s="21">
+        <v>500</v>
+      </c>
+      <c r="F21" s="21"/>
+      <c r="G21" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="H21" s="20" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A22" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="B22" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="C22" s="23">
+        <v>99921</v>
+      </c>
+      <c r="D22" s="21">
+        <v>50500</v>
+      </c>
+      <c r="E22" s="21">
+        <v>55</v>
+      </c>
+      <c r="F22" s="21"/>
+      <c r="G22" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="H22" s="20"/>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A23" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="B23" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="C23" s="23">
+        <v>99976</v>
+      </c>
+      <c r="D23" s="21">
+        <v>68</v>
+      </c>
+      <c r="E23" s="21">
+        <v>44</v>
+      </c>
+      <c r="F23" s="21"/>
+      <c r="G23" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="H23" s="20"/>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A24" s="27" t="s">
+        <v>7</v>
+      </c>
+      <c r="B24" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="C24" s="25">
+        <v>99983</v>
+      </c>
+      <c r="D24" s="26">
+        <v>123</v>
+      </c>
+      <c r="E24" s="26">
+        <v>123</v>
+      </c>
+      <c r="F24" s="26">
+        <v>7</v>
+      </c>
+      <c r="G24" s="24" t="s">
+        <v>4</v>
+      </c>
+      <c r="H24" s="27"/>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A25" s="20" t="s">
+        <v>46</v>
+      </c>
+      <c r="B25" s="18" t="s">
+        <v>50</v>
+      </c>
+      <c r="C25" s="19" t="s">
+        <v>151</v>
+      </c>
+      <c r="D25" s="21">
+        <v>798</v>
+      </c>
+      <c r="E25" s="21">
+        <v>0</v>
+      </c>
+      <c r="F25" s="21"/>
+      <c r="G25" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="H25" s="20" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A28" s="28" t="s">
+        <v>155</v>
+      </c>
+      <c r="B28" s="28"/>
+      <c r="C28" s="28"/>
+      <c r="D28" s="28"/>
+      <c r="E28" s="28"/>
+      <c r="F28" s="28"/>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A29" s="29" t="s">
+        <v>156</v>
+      </c>
+      <c r="B29" s="29"/>
+      <c r="C29" s="29"/>
+      <c r="D29" s="29"/>
+      <c r="E29" s="29"/>
+      <c r="F29" s="29"/>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A30" s="30" t="s">
+        <v>157</v>
+      </c>
+      <c r="B30" s="30"/>
+      <c r="C30" s="30"/>
+      <c r="D30" s="30"/>
+      <c r="E30" s="30"/>
+      <c r="F30" s="30"/>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A31" s="31" t="s">
+        <v>158</v>
+      </c>
+      <c r="B31" s="31"/>
+      <c r="C31" s="31"/>
+      <c r="D31" s="31"/>
+      <c r="E31" s="31"/>
+      <c r="F31" s="31"/>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A32" s="32" t="s">
+        <v>159</v>
+      </c>
+      <c r="B32" s="32"/>
+      <c r="C32" s="32"/>
+      <c r="D32" s="32"/>
+      <c r="E32" s="32"/>
+      <c r="F32" s="32"/>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A33" s="33" t="s">
+        <v>160</v>
+      </c>
+      <c r="B33" s="33"/>
+      <c r="C33" s="33"/>
+      <c r="D33" s="33"/>
+      <c r="E33" s="33"/>
+      <c r="F33" s="33"/>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A39" s="34" t="s">
+        <v>154</v>
+      </c>
+      <c r="B39" s="34"/>
+      <c r="C39" s="35" t="s">
+        <v>161</v>
+      </c>
+      <c r="D39" s="36" t="s">
+        <v>162</v>
+      </c>
+      <c r="E39" s="36"/>
+      <c r="F39" s="36"/>
+      <c r="G39" s="36"/>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A40" s="37" t="s">
+        <v>60</v>
+      </c>
+      <c r="B40" s="37"/>
+      <c r="C40" s="38">
+        <v>5343</v>
+      </c>
+      <c r="D40" s="39"/>
+      <c r="E40" s="39"/>
+      <c r="F40" s="39"/>
+      <c r="G40" s="39"/>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A41" s="37" t="s">
+        <v>127</v>
+      </c>
+      <c r="B41" s="37"/>
+      <c r="C41" s="38">
+        <v>204</v>
+      </c>
+      <c r="D41" s="39" t="s">
+        <v>128</v>
+      </c>
+      <c r="E41" s="39"/>
+      <c r="F41" s="39"/>
+      <c r="G41" s="39"/>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A42" s="37" t="s">
+        <v>117</v>
+      </c>
+      <c r="B42" s="37"/>
+      <c r="C42" s="38">
+        <v>798</v>
+      </c>
+      <c r="D42" s="39"/>
+      <c r="E42" s="39"/>
+      <c r="F42" s="39"/>
+      <c r="G42" s="39"/>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A43" s="37" t="s">
+        <v>55</v>
+      </c>
+      <c r="B43" s="37"/>
+      <c r="C43" s="38">
+        <v>52180</v>
+      </c>
+      <c r="D43" s="39"/>
+      <c r="E43" s="39"/>
+      <c r="F43" s="39"/>
+      <c r="G43" s="39"/>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A40:D43">
+    <sortCondition ref="A1:A1048576"/>
+  </sortState>
+  <mergeCells count="16">
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="D42:G42"/>
+    <mergeCell ref="A43:B43"/>
+    <mergeCell ref="D43:G43"/>
+    <mergeCell ref="A39:B39"/>
+    <mergeCell ref="D39:G39"/>
+    <mergeCell ref="A40:B40"/>
+    <mergeCell ref="D40:G40"/>
+    <mergeCell ref="A41:B41"/>
+    <mergeCell ref="D41:G41"/>
+    <mergeCell ref="A28:F28"/>
+    <mergeCell ref="A29:F29"/>
+    <mergeCell ref="A30:F30"/>
+    <mergeCell ref="A31:F31"/>
+    <mergeCell ref="A32:F32"/>
+    <mergeCell ref="A33:F33"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <headerFooter>
+    <oddHeader>&amp;R18:05 - 16/04/2025</oddHeader>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6A47EC9-6FF9-C94A-93F5-603B3A771B7A}">
   <sheetPr codeName="Sheet6"/>
   <dimension ref="A1:O25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:O25"/>
+      <selection activeCell="O25" sqref="A1:O25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4043,7 +4930,7 @@
         <v>46</v>
       </c>
       <c r="B18" t="s">
-        <v>47</v>
+        <v>163</v>
       </c>
       <c r="C18" t="s">
         <v>25</v>
@@ -4398,7 +5285,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4813409B-7228-2F49-BA7C-B95E948D09DC}">
   <sheetPr codeName="Sheet7"/>
   <dimension ref="A1:O25"/>
@@ -5171,7 +6058,7 @@
         <v>46</v>
       </c>
       <c r="B18" t="s">
-        <v>47</v>
+        <v>163</v>
       </c>
       <c r="C18" t="s">
         <v>25</v>
@@ -5526,12 +6413,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F5EC7DD-B0EB-9B41-BA63-AAF43418DED7}">
   <sheetPr codeName="Sheet8"/>
   <dimension ref="A1:O25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection sqref="A1:O25"/>
     </sheetView>
   </sheetViews>
@@ -6299,7 +7186,7 @@
         <v>46</v>
       </c>
       <c r="B18" t="s">
-        <v>47</v>
+        <v>163</v>
       </c>
       <c r="C18" t="s">
         <v>25</v>
@@ -6654,13 +7541,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3741EEE-A7B0-834D-9676-C4A7ABC54ECC}">
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:G57"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N24" sqref="N24"/>
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>